<commit_message>
feat: feature engineering hist_emprestimos
</commit_message>
<xml_diff>
--- a/dic_auxiliar.xlsx
+++ b/dic_auxiliar.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\AQUI PRA CLONAR\case_datarisk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A976D1CD-74BE-493F-AA70-C2EB560848C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD0B0B4-6FD7-49F3-9E00-7689ACB68BEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D92C70BA-F811-437E-A52B-1CE4CE977F7C}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D92C70BA-F811-437E-A52B-1CE4CE977F7C}"/>
   </bookViews>
   <sheets>
     <sheet name="dicionario_dados" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dicionario_dados!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dicionario_dados!$A$1:$C$70</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="136">
   <si>
     <t>base</t>
   </si>
@@ -425,6 +425,12 @@
   </si>
   <si>
     <t>Número sequencial da parcela dentro do contrato</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1286,10 +1292,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4068E4C-371B-44FF-947B-94338A5AD4F9}">
-  <dimension ref="A1:C70"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:D70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1310,7 +1317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1321,7 +1328,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1339,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1354,7 +1361,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1365,7 +1372,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -1376,7 +1383,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -1387,7 +1394,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -1398,7 +1405,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -1409,7 +1416,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -1420,7 +1427,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -1431,7 +1438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
@@ -1442,7 +1449,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1453,7 +1460,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1464,7 +1471,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>3</v>
       </c>
@@ -1475,7 +1482,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -1486,7 +1493,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -1497,7 +1504,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1508,7 +1515,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>27</v>
       </c>
@@ -1519,7 +1526,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -1530,7 +1537,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1541,7 +1548,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -1552,7 +1559,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
@@ -1563,7 +1570,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1574,7 +1581,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>37</v>
       </c>
@@ -1584,8 +1591,11 @@
       <c r="C26" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -1595,8 +1605,11 @@
       <c r="C27" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -1606,8 +1619,11 @@
       <c r="C28" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1618,7 +1634,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -1629,7 +1645,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -1640,7 +1656,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1651,7 +1667,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -1662,7 +1678,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1672,8 +1688,11 @@
       <c r="C34" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1683,8 +1702,11 @@
       <c r="C35" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1695,7 +1717,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -1706,7 +1728,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1717,7 +1739,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1728,7 +1750,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -1739,7 +1761,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>37</v>
       </c>
@@ -1750,7 +1772,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>37</v>
       </c>
@@ -1761,7 +1783,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
@@ -1772,7 +1794,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -1783,7 +1805,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>37</v>
       </c>
@@ -1794,7 +1816,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>37</v>
       </c>
@@ -1805,7 +1827,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>37</v>
       </c>
@@ -1816,7 +1838,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -1827,7 +1849,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>37</v>
       </c>
@@ -1838,7 +1860,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>37</v>
       </c>
@@ -1849,7 +1871,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -1860,7 +1882,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>37</v>
       </c>
@@ -1871,7 +1893,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
@@ -1882,7 +1904,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>37</v>
       </c>
@@ -1893,7 +1915,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>37</v>
       </c>
@@ -1904,7 +1926,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>37</v>
       </c>
@@ -1915,7 +1937,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>37</v>
       </c>
@@ -1926,7 +1948,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -1937,7 +1959,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -1948,7 +1970,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>37</v>
       </c>
@@ -1958,8 +1980,11 @@
       <c r="C60" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>37</v>
       </c>
@@ -1970,7 +1995,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>37</v>
       </c>
@@ -1981,7 +2006,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>84</v>
       </c>
@@ -1992,7 +2017,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>84</v>
       </c>
@@ -2003,7 +2028,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -2014,7 +2039,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>84</v>
       </c>
@@ -2025,7 +2050,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>84</v>
       </c>
@@ -2036,7 +2061,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>84</v>
       </c>
@@ -2047,7 +2072,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>84</v>
       </c>
@@ -2058,7 +2083,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>84</v>
       </c>
@@ -2070,7 +2095,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{E4068E4C-371B-44FF-947B-94338A5AD4F9}"/>
+  <autoFilter ref="A1:C70" xr:uid="{E4068E4C-371B-44FF-947B-94338A5AD4F9}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="historico_emprestimos"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>